<commit_message>
updates to storyline standoff
</commit_message>
<xml_diff>
--- a/Storyline/Standoff lists all storyline inProgress.xlsx
+++ b/Storyline/Standoff lists all storyline inProgress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Kitab QNL\Data Github\DSP-Data\Storyline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BAD324-3583-4008-A789-79C2BFEC5A5C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FB7EF3-4BF3-4712-BC79-80E4D95B222B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{4C6151D0-EBB0-46DA-B22C-A46696905C77}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C6151D0-EBB0-46DA-B22C-A46696905C77}"/>
   </bookViews>
   <sheets>
     <sheet name="Mubtada" sheetId="1" r:id="rId1"/>
@@ -1640,11 +1640,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2814,7 +2814,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2:K22"/>
     </sheetView>
   </sheetViews>

</xml_diff>